<commit_message>
Completed toy model with random NPV calculations
</commit_message>
<xml_diff>
--- a/sbp-abm-survey/toy-abm/sbp-toy-abm/data/FarmsData.xlsx
+++ b/sbp-abm-survey/toy-abm/sbp-toy-abm/data/FarmsData.xlsx
@@ -409,7 +409,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Sown Permanent Pasture</t>
+          <t>Natural Pasture</t>
         </is>
       </c>
     </row>
@@ -424,7 +424,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Sown Permanent Pasture</t>
+          <t>Natural Pasture</t>
         </is>
       </c>
     </row>
@@ -454,7 +454,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Sown Permanent Pasture</t>
+          <t>Natural Pasture</t>
         </is>
       </c>
     </row>
@@ -469,7 +469,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Sown Permanent Pasture</t>
+          <t>Natural Pasture</t>
         </is>
       </c>
     </row>
@@ -484,7 +484,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Sown Permanent Pasture</t>
+          <t>Natural Pasture</t>
         </is>
       </c>
     </row>
@@ -499,7 +499,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Sown Permanent Pasture</t>
+          <t>Natural Pasture</t>
         </is>
       </c>
     </row>
@@ -529,7 +529,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Sown Permanent Pasture</t>
+          <t>Natural Pasture</t>
         </is>
       </c>
     </row>
@@ -544,7 +544,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Sown Permanent Pasture</t>
+          <t>Natural Pasture</t>
         </is>
       </c>
     </row>
@@ -589,7 +589,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Sown Permanent Pasture</t>
+          <t>Natural Pasture</t>
         </is>
       </c>
     </row>
@@ -604,7 +604,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Sown Permanent Pasture</t>
+          <t>Natural Pasture</t>
         </is>
       </c>
     </row>
@@ -619,7 +619,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Sown Permanent Pasture</t>
+          <t>Natural Pasture</t>
         </is>
       </c>
     </row>
@@ -634,7 +634,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Sown Permanent Pasture</t>
+          <t>Natural Pasture</t>
         </is>
       </c>
     </row>
@@ -739,7 +739,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Sown Permanent Pasture</t>
+          <t>Natural Pasture</t>
         </is>
       </c>
     </row>
@@ -784,7 +784,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Sown Permanent Pasture</t>
+          <t>Natural Pasture</t>
         </is>
       </c>
     </row>
@@ -799,7 +799,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Sown Permanent Pasture</t>
+          <t>Natural Pasture</t>
         </is>
       </c>
     </row>
@@ -814,7 +814,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Sown Permanent Pasture</t>
+          <t>Natural Pasture</t>
         </is>
       </c>
     </row>
@@ -829,7 +829,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Sown Permanent Pasture</t>
+          <t>Natural Pasture</t>
         </is>
       </c>
     </row>

</xml_diff>